<commit_message>
Hooks, BDD Screenshot, Looger
</commit_message>
<xml_diff>
--- a/src/main/resources/testcase/TestCase.xlsx
+++ b/src/main/resources/testcase/TestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdnas/eclipse-workspace/bdd.geico/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdnas/eclipse-workspace/bdd.geico/src/main/resources/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6AD9378-331B-9942-992A-D2EBD573A302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D8156D-FBFE-184B-BF6F-F9BA0B5EBBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{FFDA58D5-0B03-9B46-B5AD-EB944045C04F}"/>
   </bookViews>
@@ -301,9 +301,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -341,7 +341,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -447,7 +447,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -600,7 +600,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>